<commit_message>
Update : Player Stat 레벨 추가 및 Player HPUI 구현 중
</commit_message>
<xml_diff>
--- a/Assets/Resources/ExcelDB/UserDB.xlsx
+++ b/Assets/Resources/ExcelDB/UserDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\IdleSoul\Assets\Resources\ExcelDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D75084-1849-4AA6-B2F2-A096D677888E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8BBFF5-EFE6-4FA3-AEDE-55DE19DC3D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="35">
   <si>
     <t>key</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -79,65 +79,89 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>Gold</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Diamonds</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PlayTimeInSeconds</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>float</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>UserID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>지존감자탕</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CurChapter</t>
+  </si>
+  <si>
+    <t>CurStageNum</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CurChapter</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AtkLevel</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DefLevel</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CriticalRateLevel</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CriticalDamageLevel</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReduceDamageLevel</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>Exp</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>MaxExp</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gold</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Diamonds</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>PlayTimeInSeconds</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>int</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>float</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>float</t>
-  </si>
-  <si>
-    <t>UserID</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>지존감자탕</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CurChapter</t>
-  </si>
-  <si>
-    <t>CurStageNum</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CurChapter</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>100</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MaxHealthLevel</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -197,15 +221,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -488,30 +509,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="4.875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="7.5" customWidth="1"/>
+    <col min="6" max="6" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.75" customWidth="1"/>
+    <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.25" customWidth="1"/>
+    <col min="10" max="10" width="11.625" customWidth="1"/>
+    <col min="11" max="11" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.625" customWidth="1"/>
+    <col min="13" max="13" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.125" customWidth="1"/>
+    <col min="15" max="15" width="18.75" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -522,122 +552,158 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="O1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
@@ -646,116 +712,152 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="I3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="K3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="M3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="O3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="T3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="U3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="V3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="W3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="X3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>26</v>
+      <c r="Y3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>12345678</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
       </c>
       <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>200</v>
+      </c>
+      <c r="F4" s="2">
         <v>100</v>
       </c>
-      <c r="E4" s="2">
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2">
         <v>100</v>
       </c>
-      <c r="F4" s="2">
+      <c r="I4" s="2">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2">
         <v>10</v>
       </c>
-      <c r="G4" s="2">
-        <v>10</v>
-      </c>
-      <c r="H4" s="2">
+      <c r="K4" s="2">
+        <v>1</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1</v>
+      </c>
+      <c r="M4" s="2">
+        <v>1</v>
+      </c>
+      <c r="N4" s="2">
         <v>0</v>
       </c>
-      <c r="I4" s="2">
-        <v>1</v>
-      </c>
-      <c r="J4" s="2">
+      <c r="O4" s="2">
+        <v>1</v>
+      </c>
+      <c r="P4" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>1</v>
+      </c>
+      <c r="R4" s="2">
         <v>100</v>
       </c>
-      <c r="K4" s="2">
-        <v>1</v>
-      </c>
-      <c r="L4" s="2">
-        <v>1</v>
-      </c>
-      <c r="M4" s="2">
+      <c r="S4" s="2">
+        <v>1</v>
+      </c>
+      <c r="T4" s="2">
+        <v>1</v>
+      </c>
+      <c r="U4" s="2">
         <v>0</v>
       </c>
-      <c r="N4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="P4" s="2">
+      <c r="V4" s="2">
         <v>100</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="W4" s="2">
         <v>100</v>
       </c>
-      <c r="R4" s="2">
+      <c r="X4" s="2">
         <v>0</v>
       </c>
-      <c r="S4" s="2">
-        <v>1</v>
-      </c>
-      <c r="T4" s="2">
+      <c r="Y4" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>